<commit_message>
ADD: some details in research
</commit_message>
<xml_diff>
--- a/docs/research/experiments.xlsx
+++ b/docs/research/experiments.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="10">
   <si>
     <t>Полный перебор</t>
   </si>
@@ -49,6 +49,12 @@
   <si>
     <t>Бинарное дерево</t>
   </si>
+  <si>
+    <t>Бинарное дерево - распараллеленное</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deep &lt; </t>
+  </si>
 </sst>
 </file>
 
@@ -64,7 +70,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,8 +107,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -125,11 +137,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -163,6 +188,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -744,11 +780,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="208503632"/>
-        <c:axId val="210800312"/>
+        <c:axId val="178022640"/>
+        <c:axId val="178017936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="208503632"/>
+        <c:axId val="178022640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -868,12 +904,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210800312"/>
+        <c:crossAx val="178017936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="210800312"/>
+        <c:axId val="178017936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -993,7 +1029,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208503632"/>
+        <c:crossAx val="178022640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1664,11 +1700,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="210760224"/>
-        <c:axId val="210759832"/>
+        <c:axId val="178021072"/>
+        <c:axId val="178021856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="210760224"/>
+        <c:axId val="178021072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1782,12 +1818,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210759832"/>
+        <c:crossAx val="178021856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="210759832"/>
+        <c:axId val="178021856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1910,7 +1946,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210760224"/>
+        <c:crossAx val="178021072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2405,11 +2441,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="210759048"/>
-        <c:axId val="211334104"/>
+        <c:axId val="178022248"/>
+        <c:axId val="453891504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="210759048"/>
+        <c:axId val="178022248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2527,12 +2563,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211334104"/>
+        <c:crossAx val="453891504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="211334104"/>
+        <c:axId val="453891504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2650,7 +2686,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210759048"/>
+        <c:crossAx val="178022248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3145,11 +3181,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="211329792"/>
-        <c:axId val="211332536"/>
+        <c:axId val="453891896"/>
+        <c:axId val="453891112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="211329792"/>
+        <c:axId val="453891896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3267,12 +3303,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211332536"/>
+        <c:crossAx val="453891112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="211332536"/>
+        <c:axId val="453891112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3390,7 +3426,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211329792"/>
+        <c:crossAx val="453891896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3467,6 +3503,934 @@
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Зависимость</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t> от глубины</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$A$107:$A$114</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$B$107:$B$114</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>558</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>536</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>541</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>568</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>563</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>568</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>573</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>541</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="455897016"/>
+        <c:axId val="455895056"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="455897016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Глубина</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="455895056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="455895056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Количество кадров в секунду</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="455897016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$A$90:$A$94</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$B$90:$B$94</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5688</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1231</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>571</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>261</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>161</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="488153576"/>
+        <c:axId val="488156712"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="488153576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>ЧИСЛО ЧАСТИЦ</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="488156712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="488156712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>КОЛИЧЕСТВО КАДРОВ В СЕКУНДУ</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="488153576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -3631,6 +4595,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="237">
   <cs:axisTitle>
@@ -5177,6 +6221,1038 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5814,6 +7890,66 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>23811</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>252412</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Диаграмма 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6080,10 +8216,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F83"/>
+  <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6714,7 +8850,7 @@
         <v>6589</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>4</v>
       </c>
@@ -6734,7 +8870,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>1000</v>
       </c>
@@ -6750,11 +8886,12 @@
       <c r="E79" s="9">
         <v>6447</v>
       </c>
-      <c r="F79" s="4">
+      <c r="F79" s="19">
         <v>6589</v>
       </c>
+      <c r="G79" s="15"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>5000</v>
       </c>
@@ -6770,11 +8907,12 @@
       <c r="E80" s="10">
         <v>1049</v>
       </c>
-      <c r="F80" s="4">
+      <c r="F80" s="19">
         <v>970</v>
       </c>
+      <c r="G80" s="15"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>10000</v>
       </c>
@@ -6790,11 +8928,12 @@
       <c r="E81" s="10">
         <v>365</v>
       </c>
-      <c r="F81" s="4">
+      <c r="F81" s="19">
         <v>405</v>
       </c>
+      <c r="G81" s="15"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>20000</v>
       </c>
@@ -6810,11 +8949,12 @@
       <c r="E82" s="10">
         <v>152</v>
       </c>
-      <c r="F82" s="4">
+      <c r="F82" s="19">
         <v>139</v>
       </c>
+      <c r="G82" s="15"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>30000</v>
       </c>
@@ -6830,9 +8970,159 @@
       <c r="E83" s="10">
         <v>112</v>
       </c>
-      <c r="F83" s="4">
+      <c r="F83" s="19">
         <v>102</v>
       </c>
+      <c r="G83" s="15"/>
+    </row>
+    <row r="89" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B90" s="9">
+        <v>5688</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="3">
+        <v>5000</v>
+      </c>
+      <c r="B91" s="9">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="3">
+        <v>10000</v>
+      </c>
+      <c r="B92" s="9">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="3">
+        <v>20000</v>
+      </c>
+      <c r="B93" s="9">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="3">
+        <v>30000</v>
+      </c>
+      <c r="B94" s="9">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="3">
+        <v>2</v>
+      </c>
+      <c r="B107" s="9">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="3">
+        <v>3</v>
+      </c>
+      <c r="B108" s="9">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="3">
+        <v>4</v>
+      </c>
+      <c r="B109" s="9">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="3">
+        <v>5</v>
+      </c>
+      <c r="B110" s="9">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="3">
+        <v>6</v>
+      </c>
+      <c r="B111" s="9">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="3">
+        <v>7</v>
+      </c>
+      <c r="B112" s="9">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="3">
+        <v>8</v>
+      </c>
+      <c r="B113" s="9">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="3">
+        <v>9</v>
+      </c>
+      <c r="B114" s="16">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B115" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B116" s="15"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B117" s="15"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B118" s="15"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B119" s="15"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B120" s="15"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B121" s="15"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B122" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ADD: other part of research
</commit_message>
<xml_diff>
--- a/docs/research/experiments.xlsx
+++ b/docs/research/experiments.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="17">
   <si>
     <t>Полный перебор</t>
   </si>
@@ -53,16 +53,55 @@
     <t>Бинарное дерево - распараллеленное</t>
   </si>
   <si>
-    <t xml:space="preserve">deep &lt; </t>
+    <t>РАСПАРАЛЛЕЛЕННЫЕ АЛГОРИТМЫ</t>
+  </si>
+  <si>
+    <t>----</t>
+  </si>
+  <si>
+    <t>deep</t>
+  </si>
+  <si>
+    <t>Выбор числа частиц, при котором происходит деление пространства на прямоугольники</t>
+  </si>
+  <si>
+    <t>Зависимость количества кадров в секунду от количества частиц (от 10 до 100)</t>
+  </si>
+  <si>
+    <t>Зависимость количества кадров в секунду от количества частиц (от 100 до 1000)</t>
+  </si>
+  <si>
+    <t>Зависимость количества кадров в секунду от количества частиц                           (от 1000 до 30 000)</t>
+  </si>
+  <si>
+    <t>Выявление наиболее оптимальной глубины, на которой создаются потоки</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -114,7 +153,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -150,11 +189,147 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -191,14 +366,103 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -255,7 +519,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="ru-RU" baseline="0"/>
-              <a:t> 100 ДО 1000 ШАРИКОВ</a:t>
+              <a:t> 100 ДО 1000 ЧАСТИЦ</a:t>
             </a:r>
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
@@ -300,6 +564,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$B$53</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Полный перебор</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="flat" cmpd="dbl" algn="ctr">
               <a:solidFill>
@@ -395,6 +670,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$C$53</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Дерево</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
@@ -490,6 +776,17 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$D$53</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Дерево с динамическим центром</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
@@ -585,6 +882,17 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$E$53</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Дерево с 9 узлами</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
@@ -680,6 +988,17 @@
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$F$53</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Бинарное дерево</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
@@ -780,11 +1099,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="178022640"/>
-        <c:axId val="178017936"/>
+        <c:axId val="203626472"/>
+        <c:axId val="203627888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="178022640"/>
+        <c:axId val="203626472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -904,12 +1223,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="178017936"/>
+        <c:crossAx val="203627888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="178017936"/>
+        <c:axId val="203627888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1029,7 +1348,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="178022640"/>
+        <c:crossAx val="203626472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1048,9 +1367,7 @@
       <c:spPr>
         <a:noFill/>
         <a:ln cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="accent2"/>
-          </a:solidFill>
+          <a:noFill/>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -1127,7 +1444,44 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Зависимость</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t> количества кадров в секунду от количества частиц, при котором происходит деление пространства</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.38646120082201352"/>
+          <c:y val="2.0136639215300765E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1166,6 +1520,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Полный перебор</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -1273,6 +1638,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Дерево</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -1377,6 +1753,17 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Дерево с динамическим центром</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -1481,6 +1868,17 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Дерево с 9 узлами</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -1588,6 +1986,17 @@
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Бинарное дерево</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -1700,11 +2109,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="178021072"/>
-        <c:axId val="178021856"/>
+        <c:axId val="203947696"/>
+        <c:axId val="203945736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="178021072"/>
+        <c:axId val="203947696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1744,7 +2153,15 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>КОЛИЧЕСТВО ЧАСТИЦ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t>, </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
                   <a:t>n</a:t>
                 </a:r>
                 <a:endParaRPr lang="ru-RU"/>
@@ -1818,12 +2235,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="178021856"/>
+        <c:crossAx val="203945736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="178021856"/>
+        <c:axId val="203945736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1863,12 +2280,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="ru-RU"/>
-                  <a:t>Количество</a:t>
-                </a:r>
-                <a:r>
                   <a:rPr lang="ru-RU" baseline="0"/>
-                  <a:t> кадров в секунду</a:t>
+                  <a:t>КОЛИЧЕСТВО КАДРОВ В СЕКУНДУ</a:t>
                 </a:r>
               </a:p>
               <a:p>
@@ -1946,7 +2359,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="178021072"/>
+        <c:crossAx val="203947696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2066,7 +2479,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="ru-RU" baseline="0"/>
-              <a:t> 10 ДО 100 ШАРИКОВ</a:t>
+              <a:t> 10 ДО 100 ЧАСТИЦ</a:t>
             </a:r>
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
@@ -2111,6 +2524,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$B$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Полный перебор</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -2176,6 +2600,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$C$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Дерево</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -2241,6 +2676,17 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$D$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Дерево с динамическим центром</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -2306,6 +2752,17 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$E$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Дерево с 9 узлами</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -2371,6 +2828,17 @@
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$F$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Бинарное дерево</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -2441,11 +2909,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="178022248"/>
-        <c:axId val="453891504"/>
+        <c:axId val="203944560"/>
+        <c:axId val="203944952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="178022248"/>
+        <c:axId val="203944560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2563,12 +3031,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="453891504"/>
+        <c:crossAx val="203944952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="453891504"/>
+        <c:axId val="203944952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2686,7 +3154,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="178022248"/>
+        <c:crossAx val="203944560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2806,7 +3274,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="ru-RU" baseline="0"/>
-              <a:t> 1 000 ДО 30 000 ШАРИКОВ</a:t>
+              <a:t> 1 000 ДО 30 000 ЧАСТИЦ</a:t>
             </a:r>
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
@@ -2851,6 +3319,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$B$78</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Полный перебор</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -2916,6 +3395,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$C$78</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Дерево</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -2981,6 +3471,17 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$D$78</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Дерево с динамическим центром</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -3046,6 +3547,17 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$E$78</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Дерево с 9 узлами</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -3111,6 +3623,17 @@
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$F$78</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Бинарное дерево</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -3181,11 +3704,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="453891896"/>
-        <c:axId val="453891112"/>
+        <c:axId val="203946128"/>
+        <c:axId val="203946912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="453891896"/>
+        <c:axId val="203946128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3303,12 +3826,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="453891112"/>
+        <c:crossAx val="203946912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="453891112"/>
+        <c:axId val="203946912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3426,7 +3949,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="453891896"/>
+        <c:crossAx val="203946128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3638,33 +4161,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$B$107:$B$114</c:f>
+              <c:f>Лист1!$D$107:$D$114</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>558</c:v>
+                  <c:v>1398</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>536</c:v>
+                  <c:v>1310</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>541</c:v>
+                  <c:v>1179</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>568</c:v>
+                  <c:v>1280</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>563</c:v>
+                  <c:v>1284</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>568</c:v>
+                  <c:v>1169</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>573</c:v>
+                  <c:v>1196</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>541</c:v>
+                  <c:v>1327</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3679,11 +4202,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="455897016"/>
-        <c:axId val="455895056"/>
+        <c:axId val="204453200"/>
+        <c:axId val="204453592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="455897016"/>
+        <c:axId val="204453200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3796,12 +4319,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455895056"/>
+        <c:crossAx val="204453592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="455895056"/>
+        <c:axId val="204453592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3914,7 +4437,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455897016"/>
+        <c:crossAx val="204453200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4010,6 +4533,103 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>ОТ 1 000 ДО 30 </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>000 ЧАСТИЦ </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>(РАСПАРАЛЛЕЛЕННЫЕ АЛГОРИТМЫ)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -4023,13 +4643,27 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:schemeClr>
+                </a:sysClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -4047,8 +4681,407 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="5"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$B$90</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Полный перебор</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$A$91:$A$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$B$91:$B$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$C$90</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Дерево</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$A$91:$A$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$C$91:$C$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>713</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$D$90</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Дерево с динамическим центром</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$A$91:$A$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$D$91:$D$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1116</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>841</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>484</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>226</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$E$90</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Дерево с 9 узлами</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$A$91:$A$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$E$91:$E$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>572</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>532</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>181</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$F$90</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Бинарное дерево</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$A$91:$A$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$F$91:$F$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>771</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>317</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>283</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$B$90</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Полный перебор</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -4063,7 +5096,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Лист1!$A$90:$A$94</c:f>
+              <c:f>Лист1!$A$91:$A$95</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4087,24 +5120,328 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$B$90:$B$94</c:f>
+              <c:f>Лист1!$B$91:$B$95</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5688</c:v>
+                  <c:v>730</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1231</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>571</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>261</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>161</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$C$90</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Дерево</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$A$91:$A$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$C$91:$C$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>713</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$D$90</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Дерево с динамическим центром</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$A$91:$A$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$D$91:$D$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1116</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>841</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>484</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>226</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$E$90</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Дерево с 9 узлами</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$A$91:$A$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$E$91:$E$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>572</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>532</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>181</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$F$90</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Бинарное дерево</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$A$91:$A$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$F$91:$F$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>771</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>317</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>283</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4119,11 +5456,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="488153576"/>
-        <c:axId val="488156712"/>
+        <c:axId val="393573688"/>
+        <c:axId val="393574080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="488153576"/>
+        <c:axId val="393573688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4236,14 +5573,837 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="488156712"/>
+        <c:crossAx val="393574080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="488156712"/>
+        <c:axId val="393574080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1200"/>
+          <c:min val="-200"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>КОЛИЧЕСТВО</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t> КАДРОВ В СЕКУНДУ</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="393573688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="4"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>ОТ 1 000 ДО 30 000 ЧАСТИЦ (РАСПАРАЛЛЕЛЕННЫЕ АЛГОРИТМЫ) - </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" sz="1200"/>
+              <a:t>в</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" sz="1200" baseline="0"/>
+              <a:t> масштабе, соизмеримом с тем, который используется с нераспараллеленными алгоритмами</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU" sz="1200"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$B$90</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Полный перебор</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$A$91:$A$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$B$91:$B$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$C$90</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Дерево</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$A$91:$A$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$C$91:$C$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>713</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$D$90</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Дерево с динамическим центром</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$A$91:$A$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$D$91:$D$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1116</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>841</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>484</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>226</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$E$90</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Дерево с 9 узлами</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$A$91:$A$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$E$91:$E$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>572</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>532</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>181</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$F$90</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Бинарное дерево</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$A$91:$A$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$F$91:$F$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>771</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>317</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>283</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="396805064"/>
+        <c:axId val="495114040"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="396805064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>ЧИСЛО</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t> ЧАСТИЦ</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="495114040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="495114040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="9000"/>
+          <c:min val="-1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4354,7 +6514,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="488153576"/>
+        <c:crossAx val="396805064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4675,6 +6835,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="237">
   <cs:axisTitle>
@@ -7253,6 +9453,522 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7773,13 +10489,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>9526</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
       <xdr:row>70</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
@@ -7808,8 +10524,8 @@
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>157163</xdr:rowOff>
     </xdr:to>
@@ -7838,8 +10554,8 @@
       <xdr:rowOff>176211</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
@@ -7863,13 +10579,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
+      <xdr:colOff>9523</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>-1</xdr:colOff>
       <xdr:row>99</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
@@ -7922,20 +10638,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>252412</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>7790</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>173614</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>149802</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Диаграмма 6"/>
+        <xdr:cNvPr id="8" name="Диаграмма 7"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7945,6 +10661,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>165386</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>20347</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>155864</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>6060</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Диаграмма 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8216,10 +10962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G122"/>
+  <dimension ref="A1:G128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8230,24 +10976,33 @@
     <col min="6" max="6" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="1:6" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="30"/>
+    </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="27" t="s">
         <v>7</v>
       </c>
     </row>
@@ -8507,20 +11262,31 @@
         <v>70</v>
       </c>
     </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="33"/>
+    </row>
     <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="27" t="s">
         <v>7</v>
       </c>
     </row>
@@ -8623,6 +11389,17 @@
       <c r="F33" s="4">
         <v>106847</v>
       </c>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" s="32"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="33"/>
     </row>
     <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
@@ -8850,6 +11627,25 @@
         <v>6589</v>
       </c>
     </row>
+    <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B76" s="36"/>
+      <c r="C76" s="36"/>
+      <c r="D76" s="36"/>
+      <c r="E76" s="36"/>
+      <c r="F76" s="37"/>
+    </row>
+    <row r="77" spans="1:7" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="38"/>
+      <c r="B77" s="34"/>
+      <c r="C77" s="34"/>
+      <c r="D77" s="34"/>
+      <c r="E77" s="34"/>
+      <c r="F77" s="39"/>
+    </row>
     <row r="78" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>4</v>
@@ -8886,7 +11682,7 @@
       <c r="E79" s="9">
         <v>6447</v>
       </c>
-      <c r="F79" s="19">
+      <c r="F79" s="4">
         <v>6589</v>
       </c>
       <c r="G79" s="15"/>
@@ -8907,7 +11703,7 @@
       <c r="E80" s="10">
         <v>1049</v>
       </c>
-      <c r="F80" s="19">
+      <c r="F80" s="4">
         <v>970</v>
       </c>
       <c r="G80" s="15"/>
@@ -8928,7 +11724,7 @@
       <c r="E81" s="10">
         <v>365</v>
       </c>
-      <c r="F81" s="19">
+      <c r="F81" s="4">
         <v>405</v>
       </c>
       <c r="G81" s="15"/>
@@ -8949,7 +11745,7 @@
       <c r="E82" s="10">
         <v>152</v>
       </c>
-      <c r="F82" s="19">
+      <c r="F82" s="4">
         <v>139</v>
       </c>
       <c r="G82" s="15"/>
@@ -8970,161 +11766,462 @@
       <c r="E83" s="10">
         <v>112</v>
       </c>
-      <c r="F83" s="19">
+      <c r="F83" s="4">
         <v>102</v>
       </c>
       <c r="G83" s="15"/>
     </row>
-    <row r="89" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A89" s="4" t="s">
+    <row r="86" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="87" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B87" s="41"/>
+      <c r="C87" s="41"/>
+      <c r="D87" s="41"/>
+      <c r="E87" s="41"/>
+      <c r="F87" s="42"/>
+    </row>
+    <row r="88" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B88" s="36"/>
+      <c r="C88" s="36"/>
+      <c r="D88" s="36"/>
+      <c r="E88" s="36"/>
+      <c r="F88" s="37"/>
+    </row>
+    <row r="89" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="38"/>
+      <c r="B89" s="34"/>
+      <c r="C89" s="34"/>
+      <c r="D89" s="34"/>
+      <c r="E89" s="34"/>
+      <c r="F89" s="39"/>
+    </row>
+    <row r="90" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A90" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="3">
-        <v>1000</v>
-      </c>
-      <c r="B90" s="9">
-        <v>5688</v>
+      <c r="B90" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C90" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D90" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E90" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="F90" s="27" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="B91" s="9">
-        <v>1231</v>
+        <v>730</v>
+      </c>
+      <c r="C91" s="9">
+        <v>713</v>
+      </c>
+      <c r="D91" s="9">
+        <v>1116</v>
+      </c>
+      <c r="E91" s="9">
+        <v>572</v>
+      </c>
+      <c r="F91" s="9">
+        <v>771</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="B92" s="9">
-        <v>571</v>
+        <v>63</v>
+      </c>
+      <c r="C92" s="9">
+        <v>499</v>
+      </c>
+      <c r="D92" s="9">
+        <v>841</v>
+      </c>
+      <c r="E92" s="9">
+        <v>532</v>
+      </c>
+      <c r="F92" s="9">
+        <v>520</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="B93" s="9">
-        <v>261</v>
+        <v>43</v>
+      </c>
+      <c r="C93" s="9">
+        <v>504</v>
+      </c>
+      <c r="D93" s="9">
+        <v>484</v>
+      </c>
+      <c r="E93" s="9">
+        <v>330</v>
+      </c>
+      <c r="F93" s="9">
+        <v>317</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
+        <v>20000</v>
+      </c>
+      <c r="B94" s="9">
+        <v>10</v>
+      </c>
+      <c r="C94" s="9">
+        <v>208</v>
+      </c>
+      <c r="D94" s="9">
+        <v>230</v>
+      </c>
+      <c r="E94" s="9">
+        <v>178</v>
+      </c>
+      <c r="F94" s="9">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="3">
         <v>30000</v>
       </c>
-      <c r="B94" s="9">
-        <v>161</v>
+      <c r="B95" s="9">
+        <v>2</v>
+      </c>
+      <c r="C95" s="9">
+        <v>250</v>
+      </c>
+      <c r="D95" s="9">
+        <v>226</v>
+      </c>
+      <c r="E95" s="9">
+        <v>181</v>
+      </c>
+      <c r="F95" s="9">
+        <v>283</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="4" t="s">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F97" s="17"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F98" s="15"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F99" s="15"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F100" s="15"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F101" s="15"/>
+    </row>
+    <row r="102" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F102" s="15"/>
+    </row>
+    <row r="103" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B103" s="41"/>
+      <c r="C103" s="41"/>
+      <c r="D103" s="41"/>
+      <c r="E103" s="41"/>
+      <c r="F103" s="42"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B104" s="46"/>
+      <c r="C104" s="46"/>
+      <c r="D104" s="46"/>
+      <c r="E104" s="46"/>
+      <c r="F104" s="47"/>
+    </row>
+    <row r="105" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="48"/>
+      <c r="B105" s="49"/>
+      <c r="C105" s="49"/>
+      <c r="D105" s="49"/>
+      <c r="E105" s="49"/>
+      <c r="F105" s="50"/>
+    </row>
+    <row r="106" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B106" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C106" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D106" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="E106" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="F106" s="27" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="19">
         <v>2</v>
       </c>
-      <c r="B107" s="9">
-        <v>558</v>
+      <c r="B107" s="4">
+        <v>0</v>
+      </c>
+      <c r="C107" s="4">
+        <v>771</v>
+      </c>
+      <c r="D107" s="4">
+        <v>1398</v>
+      </c>
+      <c r="E107" s="4">
+        <v>732</v>
+      </c>
+      <c r="F107" s="21">
+        <v>853</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" s="19">
         <v>3</v>
       </c>
-      <c r="B108" s="9">
-        <v>536</v>
+      <c r="B108" s="4">
+        <v>0</v>
+      </c>
+      <c r="C108" s="4">
+        <v>758</v>
+      </c>
+      <c r="D108" s="4">
+        <v>1310</v>
+      </c>
+      <c r="E108" s="4">
+        <v>603</v>
+      </c>
+      <c r="F108" s="21">
+        <v>815</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="19">
         <v>4</v>
       </c>
-      <c r="B109" s="9">
-        <v>541</v>
+      <c r="B109" s="4">
+        <v>0</v>
+      </c>
+      <c r="C109" s="4">
+        <v>755</v>
+      </c>
+      <c r="D109" s="4">
+        <v>1179</v>
+      </c>
+      <c r="E109" s="4">
+        <v>596</v>
+      </c>
+      <c r="F109" s="21">
+        <v>820</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="19">
         <v>5</v>
       </c>
-      <c r="B110" s="9">
-        <v>568</v>
+      <c r="B110" s="4">
+        <v>0</v>
+      </c>
+      <c r="C110" s="4">
+        <v>745</v>
+      </c>
+      <c r="D110" s="4">
+        <v>1280</v>
+      </c>
+      <c r="E110" s="4">
+        <v>587</v>
+      </c>
+      <c r="F110" s="21">
+        <v>812</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="19">
         <v>6</v>
       </c>
-      <c r="B111" s="9">
-        <v>563</v>
+      <c r="B111" s="4">
+        <v>0</v>
+      </c>
+      <c r="C111" s="4">
+        <v>742</v>
+      </c>
+      <c r="D111" s="4">
+        <v>1284</v>
+      </c>
+      <c r="E111" s="4">
+        <v>590</v>
+      </c>
+      <c r="F111" s="21">
+        <v>814</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="19">
         <v>7</v>
       </c>
-      <c r="B112" s="9">
-        <v>568</v>
+      <c r="B112" s="4">
+        <v>0</v>
+      </c>
+      <c r="C112" s="4">
+        <v>795</v>
+      </c>
+      <c r="D112" s="4">
+        <v>1169</v>
+      </c>
+      <c r="E112" s="4">
+        <v>588</v>
+      </c>
+      <c r="F112" s="21">
+        <v>815</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="19">
         <v>8</v>
       </c>
-      <c r="B113" s="9">
-        <v>573</v>
+      <c r="B113" s="4">
+        <v>0</v>
+      </c>
+      <c r="C113" s="4">
+        <v>747</v>
+      </c>
+      <c r="D113" s="4">
+        <v>1196</v>
+      </c>
+      <c r="E113" s="4">
+        <v>578</v>
+      </c>
+      <c r="F113" s="21">
+        <v>812</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="19">
         <v>9</v>
       </c>
-      <c r="B114" s="16">
-        <v>541</v>
+      <c r="B114" s="4">
+        <v>0</v>
+      </c>
+      <c r="C114" s="4">
+        <v>755</v>
+      </c>
+      <c r="D114" s="4">
+        <v>1327</v>
+      </c>
+      <c r="E114" s="4">
+        <v>591</v>
+      </c>
+      <c r="F114" s="22">
+        <v>819</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="17" t="s">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B115" s="18">
-        <v>8</v>
-      </c>
+      <c r="B115" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C115" s="16"/>
+      <c r="D115" s="16"/>
+      <c r="E115" s="16"/>
+      <c r="F115" s="23"/>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B116" s="15"/>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B117" s="15"/>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B118" s="15"/>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B119" s="15"/>
+      <c r="E119" s="17"/>
+      <c r="F119" s="15"/>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B120" s="15"/>
+      <c r="E120" s="17"/>
+      <c r="F120" s="15"/>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B121" s="15"/>
+      <c r="E121" s="17"/>
+      <c r="F121" s="15"/>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B122" s="15"/>
+      <c r="E122" s="17"/>
+      <c r="F122" s="15"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E123" s="17"/>
+      <c r="F123" s="15"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E124" s="17"/>
+      <c r="F124" s="15"/>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E125" s="17"/>
+      <c r="F125" s="15"/>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E126" s="17"/>
+      <c r="F126" s="24"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E127" s="17"/>
+      <c r="F127" s="17"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E128" s="17"/>
+      <c r="F128" s="17"/>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A104:F105"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A76:F77"/>
+    <mergeCell ref="A87:F87"/>
+    <mergeCell ref="A88:F89"/>
+    <mergeCell ref="A103:F103"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>